<commit_message>
Metrix done Signed-off-by: Yunnna005 <annakovalenko0500@gmail.com>
</commit_message>
<xml_diff>
--- a/Docs/Assignment 1.xlsx
+++ b/Docs/Assignment 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna\Рабочий стол\CG\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13B45CB-F0E9-4113-850E-911A6DB65BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337134A9-4246-4C45-AFE4-457A208635BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -525,30 +525,30 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -936,8 +936,8 @@
       <xdr:rowOff>80683</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>908513</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1370</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>2034989</xdr:rowOff>
     </xdr:to>
@@ -964,6 +964,270 @@
         <a:xfrm>
           <a:off x="8525435" y="22295224"/>
           <a:ext cx="2683525" cy="1954306"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>25401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>27331</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AE2A881-60B1-5596-0D30-BF7C9E3C1701}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2451100" y="27825701"/>
+          <a:ext cx="2590800" cy="1437030"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1206500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>3409245</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D5705D4-CA81-48CE-735B-CEB071F48FF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1930400" y="29667200"/>
+          <a:ext cx="3721100" cy="3307645"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>136768</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>117231</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1267274</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>2090615</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E463E43-A2E1-ADD6-546A-0E7906C710E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2012460" y="35032462"/>
+          <a:ext cx="3709583" cy="1973384"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>156308</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>136768</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1133231</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>2585457</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE705312-2CD6-DFEE-009F-FA6A1CBE48CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2032000" y="39487230"/>
+          <a:ext cx="3556000" cy="2448689"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>653143</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>72571</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>217714</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1426672</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99A6701A-C702-C6E1-BC59-7EEFCF00F877}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12718143" y="27813000"/>
+          <a:ext cx="2521857" cy="1354101"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>52916</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>868426</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>2677583</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{681AB80D-7D41-D2A7-C48C-E0E36EC94399}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12181417" y="39444083"/>
+          <a:ext cx="3725926" cy="2624667"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1489,8 +1753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21:I21"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="72" zoomScaleNormal="10" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1514,10 +1778,10 @@
     </row>
     <row r="2" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="5"/>
-      <c r="D2" s="43" t="s">
+      <c r="D2" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="44"/>
+      <c r="E2" s="38"/>
       <c r="F2" s="8"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1529,7 +1793,7 @@
     <row r="3" spans="3:13" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="5"/>
       <c r="D3" s="35"/>
-      <c r="E3" s="37"/>
+      <c r="E3" s="36"/>
       <c r="F3" s="6"/>
       <c r="G3" s="11"/>
       <c r="H3" s="7"/>
@@ -1549,10 +1813,10 @@
     </row>
     <row r="5" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="5"/>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="44"/>
+      <c r="E5" s="38"/>
       <c r="F5" s="8"/>
       <c r="H5" s="15"/>
       <c r="I5" s="12"/>
@@ -1562,7 +1826,7 @@
     <row r="6" spans="3:13" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="5"/>
       <c r="D6" s="35"/>
-      <c r="E6" s="37"/>
+      <c r="E6" s="36"/>
       <c r="F6" s="16"/>
       <c r="G6" s="12"/>
       <c r="H6" s="15"/>
@@ -1582,10 +1846,10 @@
     </row>
     <row r="8" spans="3:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="5"/>
-      <c r="D8" s="43" t="s">
+      <c r="D8" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="44"/>
+      <c r="E8" s="38"/>
       <c r="F8" s="17"/>
       <c r="G8" s="12"/>
       <c r="H8" s="15"/>
@@ -1596,7 +1860,7 @@
     <row r="9" spans="3:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="5"/>
       <c r="D9" s="35"/>
-      <c r="E9" s="37"/>
+      <c r="E9" s="36"/>
       <c r="F9" s="17"/>
       <c r="G9" s="12"/>
       <c r="H9" s="15"/>
@@ -1616,16 +1880,16 @@
     </row>
     <row r="11" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="5"/>
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="44"/>
+      <c r="E11" s="38"/>
       <c r="F11" s="18"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="41" t="s">
+      <c r="H11" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="42"/>
+      <c r="I11" s="40"/>
       <c r="J11" s="8"/>
       <c r="L11" s="15"/>
       <c r="M11" s="12"/>
@@ -1633,11 +1897,11 @@
     <row r="12" spans="3:13" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="5"/>
       <c r="D12" s="35"/>
-      <c r="E12" s="37"/>
+      <c r="E12" s="36"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="35"/>
-      <c r="I12" s="37"/>
+      <c r="I12" s="36"/>
       <c r="J12" s="16"/>
       <c r="K12" s="12"/>
       <c r="L12" s="15"/>
@@ -1657,10 +1921,10 @@
     </row>
     <row r="14" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="5"/>
-      <c r="D14" s="43" t="s">
+      <c r="D14" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="44"/>
+      <c r="E14" s="38"/>
       <c r="F14" s="17"/>
       <c r="G14" s="12"/>
       <c r="H14" s="15"/>
@@ -1673,7 +1937,7 @@
     <row r="15" spans="3:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="5"/>
       <c r="D15" s="35"/>
-      <c r="E15" s="37"/>
+      <c r="E15" s="36"/>
       <c r="F15" s="17"/>
       <c r="G15" s="12"/>
       <c r="H15" s="15"/>
@@ -1697,10 +1961,10 @@
     </row>
     <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="5"/>
-      <c r="D17" s="43" t="s">
+      <c r="D17" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="44"/>
+      <c r="E17" s="38"/>
       <c r="F17" s="18"/>
       <c r="G17" s="12"/>
       <c r="H17" s="15"/>
@@ -1713,7 +1977,7 @@
     <row r="18" spans="1:13" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="5"/>
       <c r="D18" s="35"/>
-      <c r="E18" s="37"/>
+      <c r="E18" s="36"/>
       <c r="F18" s="20"/>
       <c r="H18" s="15"/>
       <c r="I18" s="12"/>
@@ -1734,18 +1998,18 @@
     </row>
     <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="5"/>
-      <c r="D20" s="43" t="s">
+      <c r="D20" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="44"/>
-      <c r="F20" s="38" t="s">
+      <c r="E20" s="38"/>
+      <c r="F20" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="40"/>
-      <c r="H20" s="41" t="s">
+      <c r="G20" s="42"/>
+      <c r="H20" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="I20" s="42"/>
+      <c r="I20" s="40"/>
       <c r="J20" s="17"/>
       <c r="K20" s="12"/>
       <c r="L20" s="15"/>
@@ -1754,11 +2018,11 @@
     <row r="21" spans="1:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="5"/>
       <c r="D21" s="35"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="40"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="42"/>
       <c r="H21" s="35"/>
-      <c r="I21" s="37"/>
+      <c r="I21" s="36"/>
       <c r="J21" s="17"/>
       <c r="K21" s="12"/>
       <c r="L21" s="15"/>
@@ -1776,25 +2040,25 @@
     </row>
     <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="5"/>
-      <c r="D23" s="43" t="s">
+      <c r="D23" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="44"/>
+      <c r="E23" s="38"/>
       <c r="F23" s="9"/>
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
       <c r="J23" s="10"/>
       <c r="K23" s="18"/>
-      <c r="L23" s="41" t="s">
+      <c r="L23" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="M23" s="42"/>
+      <c r="M23" s="40"/>
     </row>
     <row r="24" spans="1:13" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="5"/>
       <c r="D24" s="35"/>
-      <c r="E24" s="37"/>
+      <c r="E24" s="36"/>
       <c r="F24" s="6"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
@@ -1802,7 +2066,7 @@
       <c r="J24" s="7"/>
       <c r="K24" s="23"/>
       <c r="L24" s="35"/>
-      <c r="M24" s="37"/>
+      <c r="M24" s="36"/>
     </row>
     <row r="25" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D25" s="13"/>
@@ -1815,10 +2079,10 @@
     <row r="26" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="C26" s="24"/>
-      <c r="D26" s="41" t="s">
+      <c r="D26" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="42"/>
+      <c r="E26" s="40"/>
       <c r="F26" s="12"/>
       <c r="J26" s="15"/>
       <c r="K26" s="12"/>
@@ -1830,7 +2094,7 @@
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
       <c r="D27" s="35"/>
-      <c r="E27" s="37"/>
+      <c r="E27" s="36"/>
       <c r="F27" s="12"/>
       <c r="J27" s="15"/>
       <c r="K27" s="12"/>
@@ -1848,15 +2112,15 @@
       <c r="M28" s="12"/>
     </row>
     <row r="29" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="42"/>
+      <c r="B29" s="40"/>
       <c r="C29" s="25"/>
-      <c r="D29" s="43" t="s">
+      <c r="D29" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="44"/>
+      <c r="E29" s="38"/>
       <c r="F29" s="9"/>
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
@@ -1868,10 +2132,10 @@
     </row>
     <row r="30" spans="1:13" ht="322.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="35"/>
-      <c r="B30" s="37"/>
+      <c r="B30" s="36"/>
       <c r="C30" s="25"/>
       <c r="D30" s="35"/>
-      <c r="E30" s="37"/>
+      <c r="E30" s="36"/>
       <c r="F30" s="20"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
@@ -1889,44 +2153,44 @@
       <c r="M31" s="8"/>
     </row>
     <row r="32" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="44"/>
+      <c r="B32" s="38"/>
       <c r="C32" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="43" t="s">
+      <c r="D32" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="44"/>
-      <c r="F32" s="38" t="s">
+      <c r="E32" s="38"/>
+      <c r="F32" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="39"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="40"/>
-      <c r="L32" s="43" t="s">
+      <c r="G32" s="44"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="44"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="M32" s="44"/>
+      <c r="M32" s="38"/>
     </row>
     <row r="33" spans="1:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="45"/>
-      <c r="B33" s="36"/>
+      <c r="B33" s="43"/>
       <c r="C33" s="17"/>
       <c r="D33" s="35"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="40"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="42"/>
       <c r="L33" s="35"/>
-      <c r="M33" s="36"/>
+      <c r="M33" s="43"/>
     </row>
     <row r="34" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
@@ -1938,33 +2202,46 @@
     </row>
     <row r="35" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C35" s="5"/>
-      <c r="D35" s="41" t="s">
+      <c r="D35" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="E35" s="42"/>
+      <c r="E35" s="40"/>
       <c r="F35" s="12"/>
     </row>
     <row r="36" spans="1:13" ht="213.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="5"/>
       <c r="D36" s="35"/>
-      <c r="E36" s="37"/>
+      <c r="E36" s="36"/>
       <c r="F36" s="12"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E38" s="26"/>
       <c r="F38" s="26"/>
       <c r="H38" s="35"/>
-      <c r="I38" s="36"/>
+      <c r="I38" s="43"/>
     </row>
     <row r="91" ht="0.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F32:K32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:K33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="L33:M33"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="H11:I11"/>
@@ -1981,25 +2258,12 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D23:E23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F32:K32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:K33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
AS1 Signed-off-by: Yunnna005 <annakovalenko0500@gmail.com>
</commit_message>
<xml_diff>
--- a/Docs/Assignment 1.xlsx
+++ b/Docs/Assignment 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna\Рабочий стол\CG\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337134A9-4246-4C45-AFE4-457A208635BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3A5653-1C64-44DD-ADE6-A63DB071173B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -415,7 +415,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -525,6 +525,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -533,27 +551,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -572,6 +573,1840 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$1:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>23.997039999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.352049999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.713570000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.447320000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.893419999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.1662</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25.534099999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25.889099999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25.250630000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24.984380000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22.430479999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21.70326</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>10.11586</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.8634280000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.9353</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.049169</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.7616810000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.6846309999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.11115</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.8681399999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1.9400120000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.0444560000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.7569679999999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.6799189999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3791-47E2-A51F-13A36E7BDEE3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="385219983"/>
+        <c:axId val="385220463"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="385219983"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="385220463"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="385220463"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="385219983"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$1:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>23.997039999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.352049999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.713570000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.447320000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.893419999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.1662</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25.534099999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25.889099999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25.250630000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24.984380000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22.430479999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21.70326</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>10.11586</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.8634280000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.9353</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.049169</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.7616810000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.6846309999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.11115</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.8681399999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1.9400120000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.0444560000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.7569679999999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.6799189999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C2EB-4272-99D1-CE49A0AA60C7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="385219983"/>
+        <c:axId val="385220463"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="385219983"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="385220463"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="385220463"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="385219983"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -893,7 +2728,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>600636</xdr:colOff>
+      <xdr:colOff>600637</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>1162714</xdr:rowOff>
     </xdr:to>
@@ -937,7 +2772,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1370</xdr:colOff>
+      <xdr:colOff>1371</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>2034989</xdr:rowOff>
     </xdr:to>
@@ -1158,8 +2993,8 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>217714</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>1426672</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>11529</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1234,6 +3069,285 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>123371</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>94343</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1076739" cy="1094146"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDB66821-FAF5-0869-A9D6-52C184186AF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="123371" y="35081029"/>
+          <a:ext cx="1076739" cy="1094146"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" b="1"/>
+            <a:t>1  0  0  0</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" b="1"/>
+            <a:t>0  1  0  0</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" b="1"/>
+            <a:t>0  0  1  0</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" b="1"/>
+            <a:t>0  0  -1 0</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>87086</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2640659" cy="2159053"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACAF13C2-42B5-90BB-64A6-0CC6F235715A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="39500629"/>
+          <a:ext cx="2640659" cy="2159053"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100"/>
+            <a:t>[23.99704 10.11586 -46.89024 -44.79855]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100"/>
+            <a:t>[24.35205 -1.863428 -47.34448 -45.25188]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100"/>
+            <a:t>[23.71357 -1.9353 -48.11723 -46.02309]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100"/>
+            <a:t>[23.44732 7.049169 -47.77655 -45.68309]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100"/>
+            <a:t>[20.89342 6.761681 -50.86755 -48.76791]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100"/>
+            <a:t>[20.1662 9.684631 -51.52674 -49.42579]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100"/>
+            <a:t>[25.5341 10.11115 -48.17671 -46.08245]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100"/>
+            <a:t>[25.8891 -1.86814 -48.63095 -46.53578]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100"/>
+            <a:t>[25.25063 -1.940012 -49.4037 -47.30699]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100"/>
+            <a:t>[24.98438 7.044456 -49.06301 -46.96699]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100"/>
+            <a:t>[22.43048 6.756968 -52.15401 -50.05181]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100"/>
+            <a:t>[21.70326 9.679919 -52.81321 -50.70968]</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>52102</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>84666</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1159282</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>2650718</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60C0AFBD-B16D-4BD0-A32F-372EDEEF4299}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22DC892B-7BB7-4D09-7CA6-804633092E13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1753,13 +3867,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="72" zoomScaleNormal="10" workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="66" zoomScaleNormal="10" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
     <col min="4" max="4" width="37.5546875" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
@@ -1778,10 +3894,10 @@
     </row>
     <row r="2" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="5"/>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="38"/>
+      <c r="E2" s="44"/>
       <c r="F2" s="8"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1793,7 +3909,7 @@
     <row r="3" spans="3:13" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="5"/>
       <c r="D3" s="35"/>
-      <c r="E3" s="36"/>
+      <c r="E3" s="37"/>
       <c r="F3" s="6"/>
       <c r="G3" s="11"/>
       <c r="H3" s="7"/>
@@ -1813,10 +3929,10 @@
     </row>
     <row r="5" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="5"/>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="38"/>
+      <c r="E5" s="44"/>
       <c r="F5" s="8"/>
       <c r="H5" s="15"/>
       <c r="I5" s="12"/>
@@ -1826,7 +3942,7 @@
     <row r="6" spans="3:13" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="5"/>
       <c r="D6" s="35"/>
-      <c r="E6" s="36"/>
+      <c r="E6" s="37"/>
       <c r="F6" s="16"/>
       <c r="G6" s="12"/>
       <c r="H6" s="15"/>
@@ -1846,10 +3962,10 @@
     </row>
     <row r="8" spans="3:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="5"/>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="38"/>
+      <c r="E8" s="44"/>
       <c r="F8" s="17"/>
       <c r="G8" s="12"/>
       <c r="H8" s="15"/>
@@ -1860,7 +3976,7 @@
     <row r="9" spans="3:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="5"/>
       <c r="D9" s="35"/>
-      <c r="E9" s="36"/>
+      <c r="E9" s="37"/>
       <c r="F9" s="17"/>
       <c r="G9" s="12"/>
       <c r="H9" s="15"/>
@@ -1880,16 +3996,16 @@
     </row>
     <row r="11" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="5"/>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="38"/>
+      <c r="E11" s="44"/>
       <c r="F11" s="18"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="39" t="s">
+      <c r="H11" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="40"/>
+      <c r="I11" s="42"/>
       <c r="J11" s="8"/>
       <c r="L11" s="15"/>
       <c r="M11" s="12"/>
@@ -1897,11 +4013,11 @@
     <row r="12" spans="3:13" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="5"/>
       <c r="D12" s="35"/>
-      <c r="E12" s="36"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="35"/>
-      <c r="I12" s="36"/>
+      <c r="I12" s="37"/>
       <c r="J12" s="16"/>
       <c r="K12" s="12"/>
       <c r="L12" s="15"/>
@@ -1921,10 +4037,10 @@
     </row>
     <row r="14" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="5"/>
-      <c r="D14" s="37" t="s">
+      <c r="D14" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="38"/>
+      <c r="E14" s="44"/>
       <c r="F14" s="17"/>
       <c r="G14" s="12"/>
       <c r="H14" s="15"/>
@@ -1937,7 +4053,7 @@
     <row r="15" spans="3:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="5"/>
       <c r="D15" s="35"/>
-      <c r="E15" s="36"/>
+      <c r="E15" s="37"/>
       <c r="F15" s="17"/>
       <c r="G15" s="12"/>
       <c r="H15" s="15"/>
@@ -1961,10 +4077,10 @@
     </row>
     <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="5"/>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="38"/>
+      <c r="E17" s="44"/>
       <c r="F17" s="18"/>
       <c r="G17" s="12"/>
       <c r="H17" s="15"/>
@@ -1977,7 +4093,7 @@
     <row r="18" spans="1:13" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="5"/>
       <c r="D18" s="35"/>
-      <c r="E18" s="36"/>
+      <c r="E18" s="37"/>
       <c r="F18" s="20"/>
       <c r="H18" s="15"/>
       <c r="I18" s="12"/>
@@ -1998,18 +4114,18 @@
     </row>
     <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="5"/>
-      <c r="D20" s="37" t="s">
+      <c r="D20" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="41" t="s">
+      <c r="E20" s="44"/>
+      <c r="F20" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="42"/>
-      <c r="H20" s="39" t="s">
+      <c r="G20" s="40"/>
+      <c r="H20" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="I20" s="40"/>
+      <c r="I20" s="42"/>
       <c r="J20" s="17"/>
       <c r="K20" s="12"/>
       <c r="L20" s="15"/>
@@ -2018,11 +4134,11 @@
     <row r="21" spans="1:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="5"/>
       <c r="D21" s="35"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="42"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="40"/>
       <c r="H21" s="35"/>
-      <c r="I21" s="36"/>
+      <c r="I21" s="37"/>
       <c r="J21" s="17"/>
       <c r="K21" s="12"/>
       <c r="L21" s="15"/>
@@ -2040,25 +4156,25 @@
     </row>
     <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="5"/>
-      <c r="D23" s="37" t="s">
+      <c r="D23" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="38"/>
+      <c r="E23" s="44"/>
       <c r="F23" s="9"/>
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
       <c r="J23" s="10"/>
       <c r="K23" s="18"/>
-      <c r="L23" s="39" t="s">
+      <c r="L23" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="M23" s="40"/>
+      <c r="M23" s="42"/>
     </row>
     <row r="24" spans="1:13" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="5"/>
       <c r="D24" s="35"/>
-      <c r="E24" s="36"/>
+      <c r="E24" s="37"/>
       <c r="F24" s="6"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
@@ -2066,7 +4182,7 @@
       <c r="J24" s="7"/>
       <c r="K24" s="23"/>
       <c r="L24" s="35"/>
-      <c r="M24" s="36"/>
+      <c r="M24" s="37"/>
     </row>
     <row r="25" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D25" s="13"/>
@@ -2079,10 +4195,10 @@
     <row r="26" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="C26" s="24"/>
-      <c r="D26" s="39" t="s">
+      <c r="D26" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="40"/>
+      <c r="E26" s="42"/>
       <c r="F26" s="12"/>
       <c r="J26" s="15"/>
       <c r="K26" s="12"/>
@@ -2094,7 +4210,7 @@
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
       <c r="D27" s="35"/>
-      <c r="E27" s="36"/>
+      <c r="E27" s="37"/>
       <c r="F27" s="12"/>
       <c r="J27" s="15"/>
       <c r="K27" s="12"/>
@@ -2112,15 +4228,15 @@
       <c r="M28" s="12"/>
     </row>
     <row r="29" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="40"/>
+      <c r="B29" s="42"/>
       <c r="C29" s="25"/>
-      <c r="D29" s="37" t="s">
+      <c r="D29" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="38"/>
+      <c r="E29" s="44"/>
       <c r="F29" s="9"/>
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
@@ -2132,10 +4248,10 @@
     </row>
     <row r="30" spans="1:13" ht="322.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="35"/>
-      <c r="B30" s="36"/>
+      <c r="B30" s="37"/>
       <c r="C30" s="25"/>
       <c r="D30" s="35"/>
-      <c r="E30" s="36"/>
+      <c r="E30" s="37"/>
       <c r="F30" s="20"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
@@ -2153,44 +4269,44 @@
       <c r="M31" s="8"/>
     </row>
     <row r="32" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="38"/>
+      <c r="B32" s="44"/>
       <c r="C32" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="37" t="s">
+      <c r="D32" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="38"/>
-      <c r="F32" s="41" t="s">
+      <c r="E32" s="44"/>
+      <c r="F32" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="G32" s="44"/>
-      <c r="H32" s="44"/>
-      <c r="I32" s="44"/>
-      <c r="J32" s="44"/>
-      <c r="K32" s="42"/>
-      <c r="L32" s="37" t="s">
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="40"/>
+      <c r="L32" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="M32" s="38"/>
+      <c r="M32" s="44"/>
     </row>
     <row r="33" spans="1:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="45"/>
-      <c r="B33" s="43"/>
+      <c r="B33" s="36"/>
       <c r="C33" s="17"/>
       <c r="D33" s="35"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="44"/>
-      <c r="H33" s="44"/>
-      <c r="I33" s="44"/>
-      <c r="J33" s="44"/>
-      <c r="K33" s="42"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="40"/>
       <c r="L33" s="35"/>
-      <c r="M33" s="43"/>
+      <c r="M33" s="36"/>
     </row>
     <row r="34" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
@@ -2202,46 +4318,33 @@
     </row>
     <row r="35" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C35" s="5"/>
-      <c r="D35" s="39" t="s">
+      <c r="D35" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="E35" s="40"/>
+      <c r="E35" s="42"/>
       <c r="F35" s="12"/>
     </row>
     <row r="36" spans="1:13" ht="213.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="5"/>
       <c r="D36" s="35"/>
-      <c r="E36" s="36"/>
+      <c r="E36" s="37"/>
       <c r="F36" s="12"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E38" s="26"/>
       <c r="F38" s="26"/>
       <c r="H38" s="35"/>
-      <c r="I38" s="43"/>
+      <c r="I38" s="36"/>
     </row>
     <row r="91" ht="0.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F32:K32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:K33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D8:E8"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="H11:I11"/>
@@ -2258,12 +4361,25 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F32:K32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:K33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:E32"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2291,13 +4407,189 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EA4FA80-9370-4F95-8930-41199F5C753B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.21875" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="46">
+        <v>23.997039999999998</v>
+      </c>
+      <c r="B1" s="46">
+        <v>10.11586</v>
+      </c>
+      <c r="C1" s="46">
+        <v>-46.890239999999999</v>
+      </c>
+      <c r="D1" s="46">
+        <v>-44.798549999999999</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="46">
+        <v>24.352049999999998</v>
+      </c>
+      <c r="B2" s="46">
+        <v>-1.8634280000000001</v>
+      </c>
+      <c r="C2" s="46">
+        <v>-47.344479999999997</v>
+      </c>
+      <c r="D2" s="46">
+        <v>-45.25188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="46">
+        <v>23.713570000000001</v>
+      </c>
+      <c r="B3" s="46">
+        <v>-1.9353</v>
+      </c>
+      <c r="C3" s="46">
+        <v>-48.117229999999999</v>
+      </c>
+      <c r="D3" s="46">
+        <v>-46.023090000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="46">
+        <v>23.447320000000001</v>
+      </c>
+      <c r="B4" s="46">
+        <v>7.049169</v>
+      </c>
+      <c r="C4" s="46">
+        <v>-47.77655</v>
+      </c>
+      <c r="D4" s="46">
+        <v>-45.68309</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="46">
+        <v>20.893419999999999</v>
+      </c>
+      <c r="B5" s="46">
+        <v>6.7616810000000003</v>
+      </c>
+      <c r="C5" s="46">
+        <v>-50.867550000000001</v>
+      </c>
+      <c r="D5" s="46">
+        <v>-48.767910000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="46">
+        <v>20.1662</v>
+      </c>
+      <c r="B6" s="46">
+        <v>9.6846309999999995</v>
+      </c>
+      <c r="C6" s="46">
+        <v>-51.526739999999997</v>
+      </c>
+      <c r="D6" s="46">
+        <v>-49.425789999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="46">
+        <v>25.534099999999999</v>
+      </c>
+      <c r="B7" s="46">
+        <v>10.11115</v>
+      </c>
+      <c r="C7" s="46">
+        <v>-48.17671</v>
+      </c>
+      <c r="D7" s="46">
+        <v>-46.082450000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="46">
+        <v>25.889099999999999</v>
+      </c>
+      <c r="B8" s="46">
+        <v>-1.8681399999999999</v>
+      </c>
+      <c r="C8" s="46">
+        <v>-48.630949999999999</v>
+      </c>
+      <c r="D8" s="46">
+        <v>-46.535780000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="46">
+        <v>25.250630000000001</v>
+      </c>
+      <c r="B9" s="46">
+        <v>-1.9400120000000001</v>
+      </c>
+      <c r="C9" s="46">
+        <v>-49.403700000000001</v>
+      </c>
+      <c r="D9" s="46">
+        <v>-47.306989999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="46">
+        <v>24.984380000000002</v>
+      </c>
+      <c r="B10" s="46">
+        <v>7.0444560000000003</v>
+      </c>
+      <c r="C10" s="46">
+        <v>-49.063009999999998</v>
+      </c>
+      <c r="D10" s="46">
+        <v>-46.966990000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="46">
+        <v>22.430479999999999</v>
+      </c>
+      <c r="B11" s="46">
+        <v>6.7569679999999996</v>
+      </c>
+      <c r="C11" s="46">
+        <v>-52.15401</v>
+      </c>
+      <c r="D11" s="46">
+        <v>-50.051810000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="46">
+        <v>21.70326</v>
+      </c>
+      <c r="B12" s="46">
+        <v>9.6799189999999999</v>
+      </c>
+      <c r="C12" s="46">
+        <v>-52.813209999999998</v>
+      </c>
+      <c r="D12" s="46">
+        <v>-50.709679999999999</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
AS1 done Signed-off-by: Yunnna005 <annakovalenko0500@gmail.com>
</commit_message>
<xml_diff>
--- a/Docs/Assignment 1.xlsx
+++ b/Docs/Assignment 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna\Рабочий стол\CG\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3A5653-1C64-44DD-ADE6-A63DB071173B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC711058-C03C-437E-AA58-7635D36F169C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment generation" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,10 @@
     <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$14:$A$25</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$14:$B$25</definedName>
+  </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -415,7 +419,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -515,6 +519,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -525,18 +530,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -545,16 +544,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -623,7 +633,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -654,98 +664,98 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$A$12</c:f>
+              <c:f>Sheet1!$A$14:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>23.997039999999998</c:v>
+                  <c:v>-0.53566555167522156</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.352049999999998</c:v>
+                  <c:v>-0.53814449256030905</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.713570000000001</c:v>
+                  <c:v>-0.51525375632101189</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.447320000000001</c:v>
+                  <c:v>-0.51326037708920302</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.893419999999999</c:v>
+                  <c:v>-0.42842557739300285</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.1662</c:v>
+                  <c:v>-0.40800966459008547</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25.534099999999999</c:v>
+                  <c:v>-0.55409597362987428</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25.889099999999999</c:v>
+                  <c:v>-0.55632676620011523</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25.250630000000001</c:v>
+                  <c:v>-0.53376107843682297</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>24.984380000000002</c:v>
+                  <c:v>-0.53195616751254449</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22.430479999999999</c:v>
+                  <c:v>-0.44814523191069411</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>21.70326</c:v>
+                  <c:v>-0.42799047440252042</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$12</c:f>
+              <c:f>Sheet1!$B$14:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>10.11586</c:v>
+                  <c:v>-0.22580775493849689</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.8634280000000001</c:v>
+                  <c:v>4.1179018418682274E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.9353</c:v>
+                  <c:v>4.2050631541689178E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.049169</c:v>
+                  <c:v>-0.15430587116589531</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.7616810000000003</c:v>
+                  <c:v>-0.13865021076359435</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.6846309999999995</c:v>
+                  <c:v>-0.19594286707405181</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.11115</c:v>
+                  <c:v>-0.21941433235429106</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1.8681399999999999</c:v>
+                  <c:v>4.0144164339783274E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-1.9400120000000001</c:v>
+                  <c:v>4.1008992540003078E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.0444560000000003</c:v>
+                  <c:v>-0.14998738475682602</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.7569679999999996</c:v>
+                  <c:v>-0.13499947354551212</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.6799189999999999</c:v>
+                  <c:v>-0.19088897819903419</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3791-47E2-A51F-13A36E7BDEE3}"/>
+              <c16:uniqueId val="{00000000-665B-42D8-A74E-F08692FA55EE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -757,11 +767,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="385219983"/>
-        <c:axId val="385220463"/>
+        <c:axId val="1346131184"/>
+        <c:axId val="1346133584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="385219983"/>
+        <c:axId val="1346131184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -818,12 +828,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385220463"/>
+        <c:crossAx val="1346133584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="385220463"/>
+        <c:axId val="1346133584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -880,7 +890,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385219983"/>
+        <c:crossAx val="1346131184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1297,6 +1307,367 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$14:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>-0.53566555167522156</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.53814449256030905</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.51525375632101189</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.51326037708920302</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.42842557739300285</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.40800966459008547</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.55409597362987428</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.55632676620011523</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.53376107843682297</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.53195616751254449</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.44814523191069411</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.42799047440252042</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$14:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>-0.22580775493849689</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1179018418682274E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2050631541689178E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.15430587116589531</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.13865021076359435</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.19594286707405181</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.21941433235429106</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.0144164339783274E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.1008992540003078E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.14998738475682602</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.13499947354551212</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.19088897819903419</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ADEB-4909-9495-010C8355FE00}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1346131184"/>
+        <c:axId val="1346133584"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1346131184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1346133584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1346133584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1346131184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1377,6 +1748,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1894,6 +2305,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3274,22 +4201,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>52102</xdr:colOff>
+      <xdr:colOff>150091</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>84666</xdr:rowOff>
+      <xdr:rowOff>46182</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1159282</xdr:colOff>
+      <xdr:colOff>1223818</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>2650718</xdr:rowOff>
+      <xdr:rowOff>2632364</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="11" name="Chart 10">
+        <xdr:cNvPr id="20" name="Chart 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60C0AFBD-B16D-4BD0-A32F-372EDEEF4299}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F115B98B-EBE4-46AA-9062-0EE5AFF2EE22}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3345,6 +4272,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE0D3DFE-8A54-A810-89DF-D22499050C74}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3642,7 +4605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -3657,24 +4620,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
       <c r="K2" s="28" t="s">
         <v>35</v>
       </c>
@@ -3867,8 +4830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="66" zoomScaleNormal="10" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36:E36"/>
+    <sheetView topLeftCell="A33" zoomScale="66" zoomScaleNormal="10" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3894,10 +4857,10 @@
     </row>
     <row r="2" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="5"/>
-      <c r="D2" s="43" t="s">
+      <c r="D2" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="44"/>
+      <c r="E2" s="39"/>
       <c r="F2" s="8"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -3908,7 +4871,7 @@
     </row>
     <row r="3" spans="3:13" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="5"/>
-      <c r="D3" s="35"/>
+      <c r="D3" s="36"/>
       <c r="E3" s="37"/>
       <c r="F3" s="6"/>
       <c r="G3" s="11"/>
@@ -3929,10 +4892,10 @@
     </row>
     <row r="5" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="5"/>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="44"/>
+      <c r="E5" s="39"/>
       <c r="F5" s="8"/>
       <c r="H5" s="15"/>
       <c r="I5" s="12"/>
@@ -3941,7 +4904,7 @@
     </row>
     <row r="6" spans="3:13" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="5"/>
-      <c r="D6" s="35"/>
+      <c r="D6" s="36"/>
       <c r="E6" s="37"/>
       <c r="F6" s="16"/>
       <c r="G6" s="12"/>
@@ -3962,10 +4925,10 @@
     </row>
     <row r="8" spans="3:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="5"/>
-      <c r="D8" s="43" t="s">
+      <c r="D8" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="44"/>
+      <c r="E8" s="39"/>
       <c r="F8" s="17"/>
       <c r="G8" s="12"/>
       <c r="H8" s="15"/>
@@ -3975,7 +4938,7 @@
     </row>
     <row r="9" spans="3:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="5"/>
-      <c r="D9" s="35"/>
+      <c r="D9" s="36"/>
       <c r="E9" s="37"/>
       <c r="F9" s="17"/>
       <c r="G9" s="12"/>
@@ -3996,27 +4959,27 @@
     </row>
     <row r="11" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="5"/>
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="44"/>
+      <c r="E11" s="39"/>
       <c r="F11" s="18"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="41" t="s">
+      <c r="H11" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="42"/>
+      <c r="I11" s="41"/>
       <c r="J11" s="8"/>
       <c r="L11" s="15"/>
       <c r="M11" s="12"/>
     </row>
     <row r="12" spans="3:13" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="5"/>
-      <c r="D12" s="35"/>
+      <c r="D12" s="36"/>
       <c r="E12" s="37"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
-      <c r="H12" s="35"/>
+      <c r="H12" s="36"/>
       <c r="I12" s="37"/>
       <c r="J12" s="16"/>
       <c r="K12" s="12"/>
@@ -4037,10 +5000,10 @@
     </row>
     <row r="14" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="5"/>
-      <c r="D14" s="43" t="s">
+      <c r="D14" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="44"/>
+      <c r="E14" s="39"/>
       <c r="F14" s="17"/>
       <c r="G14" s="12"/>
       <c r="H14" s="15"/>
@@ -4052,7 +5015,7 @@
     </row>
     <row r="15" spans="3:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="5"/>
-      <c r="D15" s="35"/>
+      <c r="D15" s="36"/>
       <c r="E15" s="37"/>
       <c r="F15" s="17"/>
       <c r="G15" s="12"/>
@@ -4077,10 +5040,10 @@
     </row>
     <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="5"/>
-      <c r="D17" s="43" t="s">
+      <c r="D17" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="44"/>
+      <c r="E17" s="39"/>
       <c r="F17" s="18"/>
       <c r="G17" s="12"/>
       <c r="H17" s="15"/>
@@ -4092,7 +5055,7 @@
     </row>
     <row r="18" spans="1:13" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="5"/>
-      <c r="D18" s="35"/>
+      <c r="D18" s="36"/>
       <c r="E18" s="37"/>
       <c r="F18" s="20"/>
       <c r="H18" s="15"/>
@@ -4114,18 +5077,18 @@
     </row>
     <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="5"/>
-      <c r="D20" s="43" t="s">
+      <c r="D20" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="44"/>
-      <c r="F20" s="38" t="s">
+      <c r="E20" s="39"/>
+      <c r="F20" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="40"/>
-      <c r="H20" s="41" t="s">
+      <c r="G20" s="43"/>
+      <c r="H20" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="I20" s="42"/>
+      <c r="I20" s="41"/>
       <c r="J20" s="17"/>
       <c r="K20" s="12"/>
       <c r="L20" s="15"/>
@@ -4133,11 +5096,11 @@
     </row>
     <row r="21" spans="1:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="5"/>
-      <c r="D21" s="35"/>
+      <c r="D21" s="36"/>
       <c r="E21" s="37"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="35"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="36"/>
       <c r="I21" s="37"/>
       <c r="J21" s="17"/>
       <c r="K21" s="12"/>
@@ -4156,24 +5119,24 @@
     </row>
     <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="5"/>
-      <c r="D23" s="43" t="s">
+      <c r="D23" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="44"/>
+      <c r="E23" s="39"/>
       <c r="F23" s="9"/>
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
       <c r="J23" s="10"/>
       <c r="K23" s="18"/>
-      <c r="L23" s="41" t="s">
+      <c r="L23" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="M23" s="42"/>
+      <c r="M23" s="41"/>
     </row>
     <row r="24" spans="1:13" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="5"/>
-      <c r="D24" s="35"/>
+      <c r="D24" s="36"/>
       <c r="E24" s="37"/>
       <c r="F24" s="6"/>
       <c r="G24" s="11"/>
@@ -4181,7 +5144,7 @@
       <c r="I24" s="11"/>
       <c r="J24" s="7"/>
       <c r="K24" s="23"/>
-      <c r="L24" s="35"/>
+      <c r="L24" s="36"/>
       <c r="M24" s="37"/>
     </row>
     <row r="25" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4195,10 +5158,10 @@
     <row r="26" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="C26" s="24"/>
-      <c r="D26" s="41" t="s">
+      <c r="D26" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="42"/>
+      <c r="E26" s="41"/>
       <c r="F26" s="12"/>
       <c r="J26" s="15"/>
       <c r="K26" s="12"/>
@@ -4209,7 +5172,7 @@
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="35"/>
+      <c r="D27" s="36"/>
       <c r="E27" s="37"/>
       <c r="F27" s="12"/>
       <c r="J27" s="15"/>
@@ -4228,15 +5191,15 @@
       <c r="M28" s="12"/>
     </row>
     <row r="29" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="42"/>
+      <c r="B29" s="41"/>
       <c r="C29" s="25"/>
-      <c r="D29" s="43" t="s">
+      <c r="D29" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="44"/>
+      <c r="E29" s="39"/>
       <c r="F29" s="9"/>
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
@@ -4247,10 +5210,10 @@
       <c r="M29" s="12"/>
     </row>
     <row r="30" spans="1:13" ht="322.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="35"/>
+      <c r="A30" s="36"/>
       <c r="B30" s="37"/>
       <c r="C30" s="25"/>
-      <c r="D30" s="35"/>
+      <c r="D30" s="36"/>
       <c r="E30" s="37"/>
       <c r="F30" s="20"/>
       <c r="G30" s="21"/>
@@ -4269,44 +5232,44 @@
       <c r="M31" s="8"/>
     </row>
     <row r="32" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="44"/>
+      <c r="B32" s="39"/>
       <c r="C32" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="43" t="s">
+      <c r="D32" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="44"/>
-      <c r="F32" s="38" t="s">
+      <c r="E32" s="39"/>
+      <c r="F32" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="39"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="40"/>
-      <c r="L32" s="43" t="s">
+      <c r="G32" s="45"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="43"/>
+      <c r="L32" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="M32" s="44"/>
+      <c r="M32" s="39"/>
     </row>
     <row r="33" spans="1:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="45"/>
-      <c r="B33" s="36"/>
+      <c r="A33" s="46"/>
+      <c r="B33" s="44"/>
       <c r="C33" s="17"/>
-      <c r="D33" s="35"/>
+      <c r="D33" s="36"/>
       <c r="E33" s="37"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="40"/>
-      <c r="L33" s="35"/>
-      <c r="M33" s="36"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="43"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="44"/>
     </row>
     <row r="34" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
@@ -4318,33 +5281,46 @@
     </row>
     <row r="35" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C35" s="5"/>
-      <c r="D35" s="41" t="s">
+      <c r="D35" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="E35" s="42"/>
+      <c r="E35" s="41"/>
       <c r="F35" s="12"/>
     </row>
     <row r="36" spans="1:13" ht="213.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="5"/>
-      <c r="D36" s="35"/>
+      <c r="D36" s="36"/>
       <c r="E36" s="37"/>
       <c r="F36" s="12"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E38" s="26"/>
       <c r="F38" s="26"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="36"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="48"/>
     </row>
     <row r="91" ht="0.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F32:K32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:K33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="L33:M33"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="H11:I11"/>
@@ -4361,25 +5337,12 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D23:E23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F32:K32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:K33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4407,10 +5370,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EA4FA80-9370-4F95-8930-41199F5C753B}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B12"/>
+      <selection activeCell="A14" sqref="A14:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4420,171 +5383,297 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="46">
+      <c r="A1" s="33">
         <v>23.997039999999998</v>
       </c>
-      <c r="B1" s="46">
+      <c r="B1" s="33">
         <v>10.11586</v>
       </c>
-      <c r="C1" s="46">
+      <c r="C1" s="33">
         <v>-46.890239999999999</v>
       </c>
-      <c r="D1" s="46">
+      <c r="D1" s="33">
         <v>-44.798549999999999</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="46">
+      <c r="A2" s="33">
         <v>24.352049999999998</v>
       </c>
-      <c r="B2" s="46">
+      <c r="B2" s="33">
         <v>-1.8634280000000001</v>
       </c>
-      <c r="C2" s="46">
+      <c r="C2" s="33">
         <v>-47.344479999999997</v>
       </c>
-      <c r="D2" s="46">
+      <c r="D2" s="33">
         <v>-45.25188</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="46">
+      <c r="A3" s="33">
         <v>23.713570000000001</v>
       </c>
-      <c r="B3" s="46">
+      <c r="B3" s="33">
         <v>-1.9353</v>
       </c>
-      <c r="C3" s="46">
+      <c r="C3" s="33">
         <v>-48.117229999999999</v>
       </c>
-      <c r="D3" s="46">
+      <c r="D3" s="33">
         <v>-46.023090000000003</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="46">
+      <c r="A4" s="33">
         <v>23.447320000000001</v>
       </c>
-      <c r="B4" s="46">
+      <c r="B4" s="33">
         <v>7.049169</v>
       </c>
-      <c r="C4" s="46">
+      <c r="C4" s="33">
         <v>-47.77655</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="33">
         <v>-45.68309</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="46">
+      <c r="A5" s="33">
         <v>20.893419999999999</v>
       </c>
-      <c r="B5" s="46">
+      <c r="B5" s="33">
         <v>6.7616810000000003</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="33">
         <v>-50.867550000000001</v>
       </c>
-      <c r="D5" s="46">
+      <c r="D5" s="33">
         <v>-48.767910000000001</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="46">
+      <c r="A6" s="33">
         <v>20.1662</v>
       </c>
-      <c r="B6" s="46">
+      <c r="B6" s="33">
         <v>9.6846309999999995</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="33">
         <v>-51.526739999999997</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="33">
         <v>-49.425789999999999</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="46">
+      <c r="A7" s="33">
         <v>25.534099999999999</v>
       </c>
-      <c r="B7" s="46">
+      <c r="B7" s="33">
         <v>10.11115</v>
       </c>
-      <c r="C7" s="46">
+      <c r="C7" s="33">
         <v>-48.17671</v>
       </c>
-      <c r="D7" s="46">
+      <c r="D7" s="33">
         <v>-46.082450000000001</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="46">
+      <c r="A8" s="33">
         <v>25.889099999999999</v>
       </c>
-      <c r="B8" s="46">
+      <c r="B8" s="33">
         <v>-1.8681399999999999</v>
       </c>
-      <c r="C8" s="46">
+      <c r="C8" s="33">
         <v>-48.630949999999999</v>
       </c>
-      <c r="D8" s="46">
+      <c r="D8" s="33">
         <v>-46.535780000000003</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="46">
+      <c r="A9" s="33">
         <v>25.250630000000001</v>
       </c>
-      <c r="B9" s="46">
+      <c r="B9" s="33">
         <v>-1.9400120000000001</v>
       </c>
-      <c r="C9" s="46">
+      <c r="C9" s="33">
         <v>-49.403700000000001</v>
       </c>
-      <c r="D9" s="46">
+      <c r="D9" s="33">
         <v>-47.306989999999999</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="46">
+      <c r="A10" s="33">
         <v>24.984380000000002</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B10" s="33">
         <v>7.0444560000000003</v>
       </c>
-      <c r="C10" s="46">
+      <c r="C10" s="33">
         <v>-49.063009999999998</v>
       </c>
-      <c r="D10" s="46">
+      <c r="D10" s="33">
         <v>-46.966990000000003</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="46">
+      <c r="A11" s="33">
         <v>22.430479999999999</v>
       </c>
-      <c r="B11" s="46">
+      <c r="B11" s="33">
         <v>6.7569679999999996</v>
       </c>
-      <c r="C11" s="46">
+      <c r="C11" s="33">
         <v>-52.15401</v>
       </c>
-      <c r="D11" s="46">
+      <c r="D11" s="33">
         <v>-50.051810000000003</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="46">
+      <c r="A12" s="33">
         <v>21.70326</v>
       </c>
-      <c r="B12" s="46">
+      <c r="B12" s="33">
         <v>9.6799189999999999</v>
       </c>
-      <c r="C12" s="46">
+      <c r="C12" s="33">
         <v>-52.813209999999998</v>
       </c>
-      <c r="D12" s="46">
+      <c r="D12" s="33">
         <v>-50.709679999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>A1/D1</f>
+        <v>-0.53566555167522156</v>
+      </c>
+      <c r="B14">
+        <f>B1/D1</f>
+        <v>-0.22580775493849689</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" ref="A15:A26" si="0">A2/D2</f>
+        <v>-0.53814449256030905</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ref="B15:B25" si="1">B2/D2</f>
+        <v>4.1179018418682274E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>-0.51525375632101189</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>4.2050631541689178E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>-0.51326037708920302</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>-0.15430587116589531</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>-0.42842557739300285</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>-0.13865021076359435</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>-0.40800966459008547</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>-0.19594286707405181</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>-0.55409597362987428</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="1"/>
+        <v>-0.21941433235429106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>-0.55632676620011523</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="1"/>
+        <v>4.0144164339783274E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>-0.53376107843682297</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="1"/>
+        <v>4.1008992540003078E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>-0.53195616751254449</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="1"/>
+        <v>-0.14998738475682602</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>-0.44814523191069411</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="1"/>
+        <v>-0.13499947354551212</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>-0.42799047440252042</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="1"/>
+        <v>-0.19088897819903419</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>